<commit_message>
Change export for classs
</commit_message>
<xml_diff>
--- a/app/views/Exports/bySelectedClassroom.xlsx
+++ b/app/views/Exports/bySelectedClassroom.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87EC003-2F96-F241-BBFF-A5B49DCEED46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="30040" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>&lt;/jx:forEach&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -61,17 +62,20 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Activity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\$#,##0.00;\-\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +105,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -201,11 +213,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -225,7 +237,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -300,6 +312,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -335,6 +364,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -510,108 +556,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="23" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18">
+    <row r="2" spans="2:5" ht="18">
       <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="2:4" ht="18">
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="2:5" ht="18">
       <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="2:5">
       <c r="B5" s="2"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="2"/>
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="B6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="12" t="s">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="5" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="7" t="s">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="C10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:5">
+      <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:5">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add absences to Export by classrooms
</commit_message>
<xml_diff>
--- a/app/views/Exports/bySelectedClassroom.xlsx
+++ b/app/views/Exports/bySelectedClassroom.xlsx
@@ -3,19 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87EC003-2F96-F241-BBFF-A5B49DCEED46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8873DBDB-F735-D84A-A43B-E2F0F2CC14C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="30040" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="3260" windowWidth="30040" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>&lt;/jx:forEach&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -65,6 +73,30 @@
   </si>
   <si>
     <t>Activity</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${absents}" var="absent"&gt;</t>
+  </si>
+  <si>
+    <t>${absent.firstname}</t>
+  </si>
+  <si>
+    <t>${absent.name}</t>
+  </si>
+  <si>
+    <t>&lt;jx:if test="${!absents.isEmpty()}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/jx:if&gt;</t>
+  </si>
+  <si>
+    <t>No absents</t>
+  </si>
+  <si>
+    <t>&lt;jx:if test="${absents.isEmpty()}"&gt;</t>
+  </si>
+  <si>
+    <t>Absences</t>
   </si>
 </sst>
 </file>
@@ -75,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="\$#,##0.00;\-\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +149,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +176,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -170,13 +215,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -213,10 +284,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,11 +640,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="132" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
@@ -579,20 +660,20 @@
         <v>10</v>
       </c>
       <c r="C2" s="9"/>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" ht="18">
       <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="2"/>
@@ -628,12 +709,12 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:5">
       <c r="C9" s="5" t="s">
@@ -663,11 +744,75 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="2:5" ht="18">
+      <c r="B15" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" s="5" customFormat="1">
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" ht="15" customHeight="1">
+      <c r="B19" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>